<commit_message>
Remove extra write_data row
</commit_message>
<xml_diff>
--- a/testfiles/ExpectedResultsTable.xlsx
+++ b/testfiles/ExpectedResultsTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\ELC3338\Spring2020\ARM-Lab\testfiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ACB6889-3504-432D-9360-E8C2A0DEA9C2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97DEFA52-0463-49A3-BE5C-AC631BF86B89}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>Instruction 1</t>
   </si>
@@ -511,29 +511,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K23"/>
+  <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="29.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.1796875" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.85546875" style="3" customWidth="1"/>
-    <col min="7" max="7" width="17.28515625" style="3" customWidth="1"/>
-    <col min="8" max="8" width="16.85546875" style="3" customWidth="1"/>
-    <col min="9" max="9" width="17.28515625" style="3" customWidth="1"/>
-    <col min="10" max="10" width="15.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.81640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.453125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.81640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.81640625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="17.26953125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="16.81640625" style="3" customWidth="1"/>
+    <col min="9" max="9" width="17.26953125" style="3" customWidth="1"/>
+    <col min="10" max="10" width="15.7265625" style="3" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="3"/>
+    <col min="12" max="16384" width="9.1796875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -566,7 +566,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>15</v>
       </c>
@@ -601,7 +601,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>30</v>
       </c>
@@ -616,7 +616,7 @@
       <c r="J3" s="7"/>
       <c r="K3" s="7"/>
     </row>
-    <row r="4" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>31</v>
       </c>
@@ -631,7 +631,7 @@
       <c r="J4" s="7"/>
       <c r="K4" s="7"/>
     </row>
-    <row r="5" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>20</v>
       </c>
@@ -646,7 +646,7 @@
       <c r="J5" s="7"/>
       <c r="K5" s="7"/>
     </row>
-    <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>21</v>
       </c>
@@ -661,7 +661,7 @@
       <c r="J6" s="7"/>
       <c r="K6" s="7"/>
     </row>
-    <row r="7" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>29</v>
       </c>
@@ -676,7 +676,7 @@
       <c r="J7" s="7"/>
       <c r="K7" s="7"/>
     </row>
-    <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>22</v>
       </c>
@@ -691,7 +691,7 @@
       <c r="J8" s="7"/>
       <c r="K8" s="7"/>
     </row>
-    <row r="9" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>23</v>
       </c>
@@ -706,7 +706,7 @@
       <c r="J9" s="7"/>
       <c r="K9" s="7"/>
     </row>
-    <row r="10" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
         <v>24</v>
       </c>
@@ -721,7 +721,7 @@
       <c r="J10" s="7"/>
       <c r="K10" s="7"/>
     </row>
-    <row r="11" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>25</v>
       </c>
@@ -736,7 +736,7 @@
       <c r="J11" s="7"/>
       <c r="K11" s="7"/>
     </row>
-    <row r="12" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
         <v>26</v>
       </c>
@@ -751,7 +751,7 @@
       <c r="J12" s="7"/>
       <c r="K12" s="7"/>
     </row>
-    <row r="13" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
         <v>27</v>
       </c>
@@ -766,7 +766,7 @@
       <c r="J13" s="7"/>
       <c r="K13" s="7"/>
     </row>
-    <row r="14" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
         <v>28</v>
       </c>
@@ -781,9 +781,9 @@
       <c r="J14" s="7"/>
       <c r="K14" s="7"/>
     </row>
-    <row r="15" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
-        <v>35</v>
+    <row r="15" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A15" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>
@@ -796,9 +796,9 @@
       <c r="J15" s="8"/>
       <c r="K15" s="8"/>
     </row>
-    <row r="16" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
@@ -811,9 +811,9 @@
       <c r="J16" s="8"/>
       <c r="K16" s="8"/>
     </row>
-    <row r="17" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
@@ -826,24 +826,24 @@
       <c r="J17" s="8"/>
       <c r="K17" s="8"/>
     </row>
-    <row r="18" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="8"/>
-      <c r="J18" s="8"/>
-      <c r="K18" s="8"/>
-    </row>
-    <row r="19" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
+      <c r="K18" s="7"/>
+    </row>
+    <row r="19" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
@@ -856,9 +856,9 @@
       <c r="J19" s="7"/>
       <c r="K19" s="7"/>
     </row>
-    <row r="20" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
@@ -871,9 +871,9 @@
       <c r="J20" s="7"/>
       <c r="K20" s="7"/>
     </row>
-    <row r="21" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
@@ -886,9 +886,9 @@
       <c r="J21" s="7"/>
       <c r="K21" s="7"/>
     </row>
-    <row r="22" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
@@ -901,21 +901,6 @@
       <c r="J22" s="7"/>
       <c r="K22" s="7"/>
     </row>
-    <row r="23" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="7"/>
-      <c r="I23" s="7"/>
-      <c r="J23" s="7"/>
-      <c r="K23" s="7"/>
-    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>